<commit_message>
MZ 14082023 update documentation TC example 2 2
</commit_message>
<xml_diff>
--- a/examples/trainData/nhanes_dict_2-1.xlsx
+++ b/examples/trainData/nhanes_dict_2-1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/examples/trainData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_0DC182E1538B0810E12D4C17052B0411797891C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C930D1-8C4C-4DE3-AE3B-7CA4957262DE}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -778,8 +784,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,13 +848,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -886,7 +900,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -920,6 +934,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -954,9 +969,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1129,14 +1145,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1176,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1210,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1251,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1279,7 +1297,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1299,7 +1317,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1322,7 +1340,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1363,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1368,7 +1386,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1391,7 +1409,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1440,7 +1458,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1481,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1483,7 +1501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1506,7 +1524,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1543,7 +1561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1563,7 +1581,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1603,7 +1621,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1695,7 +1713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1712,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1729,7 +1747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1763,7 +1781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1780,7 +1798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1797,7 +1815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1831,7 +1849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1851,7 +1869,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1871,7 +1889,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1911,7 +1929,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1931,7 +1949,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1951,7 +1969,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1971,7 +1989,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1994,7 +2012,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2014,7 +2032,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2037,7 +2055,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2060,7 +2078,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2083,7 +2101,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2106,7 +2124,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2169,7 +2187,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2192,7 +2210,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2215,7 +2233,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2238,7 +2256,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2261,7 +2279,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2284,7 +2302,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2307,7 +2325,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2330,7 +2348,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2353,7 +2371,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2376,7 +2394,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2399,7 +2417,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2419,7 +2437,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2439,7 +2457,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2462,7 +2480,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2485,7 +2503,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2508,7 +2526,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2528,7 +2546,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2571,7 +2589,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2614,7 +2632,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2637,7 +2655,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2660,7 +2678,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2680,7 +2698,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2700,7 +2718,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2720,7 +2738,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2743,7 +2761,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2766,7 +2784,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
MZ 25082023 update cleandata initialisation report
</commit_message>
<xml_diff>
--- a/examples/trainData/nhanes_dict_2-1.xlsx
+++ b/examples/trainData/nhanes_dict_2-1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/examples/trainData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_0DC182E1538B0810E12D4C17052B0411797891C7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C930D1-8C4C-4DE3-AE3B-7CA4957262DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -784,8 +778,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,21 +842,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -900,7 +886,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -934,7 +920,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -969,10 +954,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1145,16 +1129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1208,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1228,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1233,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1271,7 +1253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1279,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1299,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1340,7 +1322,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1345,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1368,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1409,7 +1391,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1432,7 +1414,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1458,7 +1440,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +1463,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1501,7 +1483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1524,7 +1506,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1544,7 +1526,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +1543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1581,7 +1563,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1601,7 +1583,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1621,7 +1603,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1644,7 +1626,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1670,7 +1652,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1696,7 +1678,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1713,7 +1695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1730,7 +1712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1747,7 +1729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1764,7 +1746,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1781,7 +1763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1798,7 +1780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1815,7 +1797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1832,7 +1814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1849,7 +1831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1869,7 +1851,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1889,7 +1871,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1909,7 +1891,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1929,7 +1911,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1949,7 +1931,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1969,7 +1951,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1989,7 +1971,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2012,7 +1994,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2032,7 +2014,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2055,7 +2037,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2078,7 +2060,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2101,7 +2083,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2124,7 +2106,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2147,7 +2129,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2167,7 +2149,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2187,7 +2169,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2192,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2233,7 +2215,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2256,7 +2238,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2279,7 +2261,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2302,7 +2284,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2325,7 +2307,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2348,7 +2330,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2371,7 +2353,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2394,7 +2376,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2417,7 +2399,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2437,7 +2419,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2457,7 +2439,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2480,7 +2462,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2503,7 +2485,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2526,7 +2508,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2546,7 +2528,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2569,7 +2551,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2589,7 +2571,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2612,7 +2594,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2632,7 +2614,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2655,7 +2637,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2678,7 +2660,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2698,7 +2680,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2718,7 +2700,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2738,7 +2720,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2761,7 +2743,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2784,7 +2766,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>84</v>
       </c>

</xml_diff>